<commit_message>
Added results of weighted occ FE
</commit_message>
<xml_diff>
--- a/results/tables/result_tracking_new.xlsx
+++ b/results/tables/result_tracking_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A2C1A7-6EA9-41BB-8319-0B67B1E4D733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDA6378-BB66-4C85-8485-9D408FA2972C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0710EB5B-6368-4E59-9B8B-91FD539FEA2D}"/>
+    <workbookView xWindow="10850" yWindow="-17510" windowWidth="17750" windowHeight="14790" xr2:uid="{0710EB5B-6368-4E59-9B8B-91FD539FEA2D}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,132 +1352,156 @@
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="G28" s="8" t="str">
+      <c r="B28">
+        <v>0.22827110292917499</v>
+      </c>
+      <c r="C28">
+        <v>0.36977136334100402</v>
+      </c>
+      <c r="D28">
+        <v>0.62817123693064103</v>
+      </c>
+      <c r="E28">
+        <v>0.37244128726772702</v>
+      </c>
+      <c r="G28" s="8">
         <f>IFERROR(C28/$B28,"")</f>
-        <v/>
-      </c>
-      <c r="H28" s="8" t="str">
+        <v>1.6198781124553112</v>
+      </c>
+      <c r="H28" s="8">
         <f t="shared" ref="H28:I30" si="32">IFERROR(D28/$B28,"")</f>
-        <v/>
-      </c>
-      <c r="I28" s="8" t="str">
+        <v>2.7518649047993686</v>
+      </c>
+      <c r="I28" s="8">
         <f t="shared" si="32"/>
-        <v/>
+        <v>1.6315743976725923</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>0</v>
       </c>
       <c r="L28" s="1">
         <f>+B28*B$3</f>
-        <v>0</v>
+        <v>0.10655727042688298</v>
       </c>
       <c r="M28" s="1">
         <f t="shared" ref="M28" si="33">+C28*C$3</f>
-        <v>0</v>
+        <v>0.25127446922188218</v>
       </c>
       <c r="N28" s="1">
         <f t="shared" ref="N28" si="34">+D28*D$3</f>
-        <v>0</v>
+        <v>0.41565770380369682</v>
       </c>
       <c r="O28" s="1">
         <f t="shared" ref="O28" si="35">+E28*E$3</f>
-        <v>0</v>
+        <v>0.2051251674695137</v>
       </c>
       <c r="P28" s="6">
         <f>+SUM(L28:O28)</f>
-        <v>0</v>
+        <v>0.97861461092197566</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="G29" s="8" t="str">
+      <c r="B29">
+        <v>0.22827110292917499</v>
+      </c>
+      <c r="C29">
+        <v>0.25326013716395901</v>
+      </c>
+      <c r="D29">
+        <v>1.01783384060056</v>
+      </c>
+      <c r="E29">
+        <v>3.4884043677039199E-2</v>
+      </c>
+      <c r="G29" s="8">
         <f t="shared" ref="G29:G30" si="36">IFERROR(C29/$B29,"")</f>
-        <v/>
-      </c>
-      <c r="H29" s="8" t="str">
+        <v>1.1094708612440414</v>
+      </c>
+      <c r="H29" s="8">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="I29" s="8" t="str">
+        <v>4.4588816873433181</v>
+      </c>
+      <c r="I29" s="8">
         <f t="shared" si="32"/>
-        <v/>
+        <v>0.15281848306424739</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L29" s="1">
         <f>+B29*B$4</f>
-        <v>0</v>
+        <v>0.10471516828046513</v>
       </c>
       <c r="M29" s="1">
         <f t="shared" ref="M29" si="37">+C29*C$4</f>
-        <v>0</v>
+        <v>0.17321922091634592</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" ref="N29" si="38">+D29*D$4</f>
-        <v>0</v>
+        <v>0.68407808338029563</v>
       </c>
       <c r="O29" s="1">
         <f t="shared" ref="O29" si="39">+E29*E$4</f>
-        <v>0</v>
+        <v>1.9785552823169301E-2</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" ref="P29:P30" si="40">+SUM(L29:O29)</f>
-        <v>0</v>
+        <v>0.98179802540027594</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="G30" s="8" t="str">
+      <c r="B30">
+        <v>0.22827110292917499</v>
+      </c>
+      <c r="C30">
+        <v>1.0766597280455901</v>
+      </c>
+      <c r="D30">
+        <v>0.113785888586552</v>
+      </c>
+      <c r="E30">
+        <v>6.0154714206556797E-2</v>
+      </c>
+      <c r="G30" s="8">
         <f t="shared" si="36"/>
-        <v/>
-      </c>
-      <c r="H30" s="8" t="str">
+        <v>4.7165835457484171</v>
+      </c>
+      <c r="H30" s="8">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="I30" s="8" t="str">
+        <v>0.49846821225486443</v>
+      </c>
+      <c r="I30" s="8">
         <f t="shared" si="32"/>
-        <v/>
+        <v>0.26352312419159257</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>1</v>
       </c>
       <c r="L30" s="1">
         <f>+B30*B$5</f>
-        <v>0</v>
+        <v>9.628360986001136E-2</v>
       </c>
       <c r="M30" s="1">
         <f t="shared" ref="M30" si="41">+C30*C$5</f>
-        <v>0</v>
+        <v>0.77373343861200294</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" ref="N30" si="42">+D30*D$5</f>
-        <v>0</v>
+        <v>7.8641944901942984E-2</v>
       </c>
       <c r="O30" s="1">
         <f t="shared" ref="O30" si="43">+E30*E$5</f>
-        <v>0</v>
+        <v>3.6760215000698725E-2</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>0.98541920837465602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>